<commit_message>
Initialized RD_RDM_WBG_w_AFOLU branch with local changes
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/_AFOLU_demand_controls.xlsx
+++ b/t3a_experiments/Experiment_1/_AFOLU_demand_controls.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-Decarb_RD/Documentos compartidos/Decarb_RD/WBG/10_RDM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\RD_RDM_test_new\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{496D3F38-63B8-4EDB-86F3-64A7B4BF2A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D71B369-37B0-41E8-9323-23937C605522}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2884EA-7AA0-4997-86EC-A9F509B75747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agr_demands" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Tech_NationalProd</t>
   </si>
@@ -36,218 +47,326 @@
     <t>Tech_Exports</t>
   </si>
   <si>
+    <t>IMPRIC</t>
+  </si>
+  <si>
+    <t>IMPBAN</t>
+  </si>
+  <si>
+    <t>IMPSGC</t>
+  </si>
+  <si>
+    <t>IMPCOC</t>
+  </si>
+  <si>
+    <t>IMPTRVEG</t>
+  </si>
+  <si>
+    <t>IMPCAF</t>
+  </si>
+  <si>
+    <t>IMPLEG</t>
+  </si>
+  <si>
+    <t>IMPROT</t>
+  </si>
+  <si>
+    <t>IMPFRT</t>
+  </si>
+  <si>
+    <t>IMPCER</t>
+  </si>
+  <si>
+    <t>IMPOTP</t>
+  </si>
+  <si>
+    <t>IMPLEC</t>
+  </si>
+  <si>
+    <t>IMPCARAVI</t>
+  </si>
+  <si>
+    <t>IMPCARBOV</t>
+  </si>
+  <si>
+    <t>IMPOTRCARPRO</t>
+  </si>
+  <si>
+    <t>IMPCARPOR</t>
+  </si>
+  <si>
+    <t>IMPOTRCAR</t>
+  </si>
+  <si>
+    <t>AG_RIC</t>
+  </si>
+  <si>
+    <t>AG_BAN</t>
+  </si>
+  <si>
+    <t>AG_SGC</t>
+  </si>
+  <si>
+    <t>AG_COC</t>
+  </si>
+  <si>
+    <t>AG_TRVEG</t>
+  </si>
+  <si>
+    <t>AG_CAF</t>
+  </si>
+  <si>
+    <t>AG_LEG</t>
+  </si>
+  <si>
+    <t>AG_ROT</t>
+  </si>
+  <si>
+    <t>AG_FRT</t>
+  </si>
+  <si>
+    <t>AGR_CER</t>
+  </si>
+  <si>
+    <t>AGR_OTP</t>
+  </si>
+  <si>
+    <t>GA_LEC</t>
+  </si>
+  <si>
+    <t>GA_CARAVI</t>
+  </si>
+  <si>
+    <t>GA_CARBOV</t>
+  </si>
+  <si>
+    <t>GA_CARPOR</t>
+  </si>
+  <si>
+    <t>GA_OTRCAR</t>
+  </si>
+  <si>
+    <t>Tech_Demand</t>
+  </si>
+  <si>
+    <t>T5SGCAGREXP</t>
+  </si>
+  <si>
+    <t>T5RICAGREXP</t>
+  </si>
+  <si>
+    <t>T5CERAGREXP</t>
+  </si>
+  <si>
+    <t>T5BANAGREXP</t>
+  </si>
+  <si>
+    <t>T5TRVEGAGREXP</t>
+  </si>
+  <si>
+    <t>T5COCAGREXP</t>
+  </si>
+  <si>
+    <t>T5LEGAGREXP</t>
+  </si>
+  <si>
+    <t>T5ROTAGREXP</t>
+  </si>
+  <si>
+    <t>T5FRTAGREXP</t>
+  </si>
+  <si>
+    <t>T5OTPAGREXP</t>
+  </si>
+  <si>
+    <t>T5CAFAGREXP</t>
+  </si>
+  <si>
+    <t>T5LECGANEXP</t>
+  </si>
+  <si>
+    <t>T5CARAVIGANEXP</t>
+  </si>
+  <si>
+    <t>T5CARBOVGANEXP</t>
+  </si>
+  <si>
+    <t>T5CARPORGANEXP</t>
+  </si>
+  <si>
+    <t>T5OTRCARPROGANEXP</t>
+  </si>
+  <si>
+    <t>T5OTRCARGANEXP</t>
+  </si>
+  <si>
+    <t>T5SGCAGR</t>
+  </si>
+  <si>
+    <t>T5RICAGR</t>
+  </si>
+  <si>
+    <t>T5CERAGR</t>
+  </si>
+  <si>
+    <t>T5BANAGR</t>
+  </si>
+  <si>
+    <t>T5TRVEGAGR</t>
+  </si>
+  <si>
+    <t>T5CAFAGR</t>
+  </si>
+  <si>
+    <t>T5COCAGR</t>
+  </si>
+  <si>
+    <t>T5LEGAGR</t>
+  </si>
+  <si>
+    <t>T5ROTAGR</t>
+  </si>
+  <si>
+    <t>T5FRTAGR</t>
+  </si>
+  <si>
+    <t>T5OTPAGR</t>
+  </si>
+  <si>
+    <t>T5LECGAN</t>
+  </si>
+  <si>
+    <t>T5CARAVIGAN</t>
+  </si>
+  <si>
+    <t>T5CARBOVGAN</t>
+  </si>
+  <si>
+    <t>T5CARPORGAN</t>
+  </si>
+  <si>
+    <t>T5OTRCARPROGAN</t>
+  </si>
+  <si>
+    <t>T5OTRCARGAN</t>
+  </si>
+  <si>
     <t>Fuel</t>
   </si>
   <si>
-    <t>IMPRIC</t>
-  </si>
-  <si>
-    <t>IMPBAN</t>
-  </si>
-  <si>
-    <t>IMPSGC</t>
-  </si>
-  <si>
-    <t>IMPCOC</t>
-  </si>
-  <si>
-    <t>IMPTRVEG</t>
-  </si>
-  <si>
-    <t>IMPCAF</t>
-  </si>
-  <si>
-    <t>IMPLEG</t>
-  </si>
-  <si>
-    <t>IMPROT</t>
-  </si>
-  <si>
-    <t>IMPFRT</t>
-  </si>
-  <si>
-    <t>IMPCER</t>
-  </si>
-  <si>
-    <t>IMPOTP</t>
-  </si>
-  <si>
-    <t>IMPLEC</t>
-  </si>
-  <si>
-    <t>IMPCARAVI</t>
-  </si>
-  <si>
-    <t>IMPCARBOV</t>
-  </si>
-  <si>
-    <t>IMPOTRCARPRO</t>
-  </si>
-  <si>
-    <t>IMPCARPOR</t>
-  </si>
-  <si>
-    <t>IMPOTRCAR</t>
+    <t>Fuel_Exports</t>
+  </si>
+  <si>
+    <t>E5AGRRIC</t>
+  </si>
+  <si>
+    <t>E5AGREXPRIC</t>
+  </si>
+  <si>
+    <t>E5AGRBAN</t>
+  </si>
+  <si>
+    <t>E5AGREXPBAN</t>
   </si>
   <si>
     <t>E5AGRSGC</t>
   </si>
   <si>
-    <t>E5AGRRIC</t>
+    <t>E5AGREXPSGC</t>
+  </si>
+  <si>
+    <t>E5AGRCOC</t>
+  </si>
+  <si>
+    <t>E5AGREXPCOC</t>
+  </si>
+  <si>
+    <t>E5AGRCAF</t>
+  </si>
+  <si>
+    <t>E5AGREXPCAF</t>
+  </si>
+  <si>
+    <t>E5AGRLEG</t>
+  </si>
+  <si>
+    <t>E5AGREXPLEG</t>
+  </si>
+  <si>
+    <t>E5AGRROT</t>
+  </si>
+  <si>
+    <t>E5AGREXPROT</t>
+  </si>
+  <si>
+    <t>E5AGRFRT</t>
+  </si>
+  <si>
+    <t>E5AGREXPFRT</t>
   </si>
   <si>
     <t>E5AGRCER</t>
   </si>
   <si>
-    <t>E5AGRBAN</t>
+    <t>E5AGREXPCER</t>
   </si>
   <si>
     <t>E5AGRTRVEG</t>
   </si>
   <si>
-    <t>E5AGRCAF</t>
-  </si>
-  <si>
-    <t>E5AGRCOC</t>
-  </si>
-  <si>
-    <t>E5AGRLEG</t>
-  </si>
-  <si>
-    <t>E5AGRROT</t>
-  </si>
-  <si>
-    <t>E5AGRFRT</t>
+    <t>E5AGREXPTRVEG</t>
   </si>
   <si>
     <t>E5AGROTP</t>
   </si>
   <si>
+    <t>E5AGREXPOTP</t>
+  </si>
+  <si>
     <t>E5GANLEC</t>
   </si>
   <si>
+    <t>E5GANEXPLEC</t>
+  </si>
+  <si>
     <t>E5GANCARAVI</t>
   </si>
   <si>
+    <t>E5GANEXPCARAVI</t>
+  </si>
+  <si>
     <t>E5GANCARBOV</t>
   </si>
   <si>
+    <t>E5GANEXPCARBOV</t>
+  </si>
+  <si>
     <t>E5GANCARPOR</t>
   </si>
   <si>
+    <t>E5GANEXPCARPOR</t>
+  </si>
+  <si>
     <t>E5GANOTRCARPRO</t>
   </si>
   <si>
+    <t>E5GANEXPOTRCARPRO</t>
+  </si>
+  <si>
     <t>E5GANOTRCAR</t>
   </si>
   <si>
-    <t>Demand Agriculture Sugar cane</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Rice</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Cereales</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Banana</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Vegetables, other</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Coffee and products</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Cocoa and products</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Legumes</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Roots</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Fruits</t>
-  </si>
-  <si>
-    <t>Demand Agriculture Other products</t>
-  </si>
-  <si>
-    <t>Demand Livestock Milk</t>
-  </si>
-  <si>
-    <t>Demand Livestock Poultry meat</t>
-  </si>
-  <si>
-    <t>Demand Livestock Beef</t>
-  </si>
-  <si>
-    <t>Demand Livestock Pork</t>
-  </si>
-  <si>
-    <t>Demand Livestock Other dairy products</t>
-  </si>
-  <si>
-    <t>Demand Livestock Other meats</t>
-  </si>
-  <si>
-    <t>E5AGREXPSGC</t>
-  </si>
-  <si>
-    <t>E5AGREXPRIC</t>
-  </si>
-  <si>
-    <t>E5AGREXPCER</t>
-  </si>
-  <si>
-    <t>E5AGREXPBAN</t>
-  </si>
-  <si>
-    <t>E5AGREXPTRVEG</t>
-  </si>
-  <si>
-    <t>E5AGREXPCOC</t>
-  </si>
-  <si>
-    <t>E5AGREXPLEG</t>
-  </si>
-  <si>
-    <t>E5AGREXPROT</t>
-  </si>
-  <si>
-    <t>E5AGREXPCAF</t>
-  </si>
-  <si>
-    <t>E5AGREXPFRT</t>
-  </si>
-  <si>
-    <t>E5AGREXPOTP</t>
-  </si>
-  <si>
-    <t>E5GANEXPLEC</t>
-  </si>
-  <si>
-    <t>E5GANEXPCARAVI</t>
-  </si>
-  <si>
-    <t>E5GANEXPCARBOV</t>
-  </si>
-  <si>
-    <t>E5GANEXPCARPOR</t>
-  </si>
-  <si>
-    <t>E5GANEXPOTRCARPRO</t>
-  </si>
-  <si>
     <t>E5GANEXPOTRCAR</t>
+  </si>
+  <si>
+    <t>GA_OTRCARPRO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,8 +391,16 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +417,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8E4BC"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -329,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -345,6 +478,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,278 +763,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.36328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7265625" customWidth="1"/>
+    <col min="7" max="7" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="F11" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="F14" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="D15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="D17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="D18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+      <c r="F18" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.45">
+      <c r="E27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,15 +1149,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -1143,6 +1379,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1154,15 +1399,30 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F3CFE0A-3B6D-4979-95EE-31CD9C47AEB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B78DEBC-D9D0-48ED-93FD-5FE5844FA749}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F3CFE0A-3B6D-4979-95EE-31CD9C47AEB2}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>